<commit_message>
Imply get csvData. TODO: set chartType
</commit_message>
<xml_diff>
--- a/yubi-backend/src/main/resources/网站数据.xlsx
+++ b/yubi-backend/src/main/resources/网站数据.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\ChatBI\ChatBI\yubi-backend\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A67D79-170D-4413-9A3D-C9B1203843DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9387021C-9B68-4DFB-8661-BE4546D11986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{229EEA6E-F8A7-2545-904A-8F0032855BE1}"/>
+    <workbookView xWindow="878" yWindow="52" windowWidth="18322" windowHeight="11348" xr2:uid="{229EEA6E-F8A7-2545-904A-8F0032855BE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -431,7 +431,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.87890625" defaultRowHeight="22.5" x14ac:dyDescent="0.6"/>
@@ -454,7 +454,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
@@ -464,7 +464,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.6">
@@ -472,7 +472,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>